<commit_message>
Update the DB structure
</commit_message>
<xml_diff>
--- a/Databases/Diseases.xlsx
+++ b/Databases/Diseases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIT\Level 6\FYP\FYP\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DF5B16-3074-4E8B-8380-FF9CE1577A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8132C9E-6FC7-4859-8D02-EF03CC4F8B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBAB22AE-A4D1-47D3-AE00-9E8D5D8FBA69}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="138">
   <si>
     <t xml:space="preserve">Diabetes </t>
   </si>
@@ -193,6 +193,261 @@
   </si>
   <si>
     <t>blood_in_sputum</t>
+  </si>
+  <si>
+    <t>Pneumonia</t>
+  </si>
+  <si>
+    <t>cough</t>
+  </si>
+  <si>
+    <t>fast_heart_rate</t>
+  </si>
+  <si>
+    <t>rusty_sputum</t>
+  </si>
+  <si>
+    <t>aching_body</t>
+  </si>
+  <si>
+    <t>feeling_confused</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>weight_gain</t>
+  </si>
+  <si>
+    <t>depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joint_pain </t>
+  </si>
+  <si>
+    <t>muscle_pain</t>
+  </si>
+  <si>
+    <t>dry_skin</t>
+  </si>
+  <si>
+    <t>swollen_extremeties</t>
+  </si>
+  <si>
+    <t>cold_hands_and_feets</t>
+  </si>
+  <si>
+    <t>enlarged_thyroid</t>
+  </si>
+  <si>
+    <t>muscle_cramps</t>
+  </si>
+  <si>
+    <t>slow_movements</t>
+  </si>
+  <si>
+    <t>slow_thoughts</t>
+  </si>
+  <si>
+    <t>abnormal_menstruation</t>
+  </si>
+  <si>
+    <t>slowed_heart_rate</t>
+  </si>
+  <si>
+    <t>Arthritis</t>
+  </si>
+  <si>
+    <t>joint_pain</t>
+  </si>
+  <si>
+    <t>stiff_neck</t>
+  </si>
+  <si>
+    <t>painful_walking</t>
+  </si>
+  <si>
+    <t>muscle_weakness</t>
+  </si>
+  <si>
+    <t>swelling_joints</t>
+  </si>
+  <si>
+    <t>movement_stiffness</t>
+  </si>
+  <si>
+    <t>inflammation_joint</t>
+  </si>
+  <si>
+    <t>warm_red_skin_over_the_affected_joint</t>
+  </si>
+  <si>
+    <t>muscle_wasting</t>
+  </si>
+  <si>
+    <t>Lower Urinary tract infection</t>
+  </si>
+  <si>
+    <t>continuous_feel_of_urine</t>
+  </si>
+  <si>
+    <t>lower_belly_pain</t>
+  </si>
+  <si>
+    <t>burning_micturition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pain_when_peeing </t>
+  </si>
+  <si>
+    <t>frequent_urination</t>
+  </si>
+  <si>
+    <t>bladder_discomfort</t>
+  </si>
+  <si>
+    <t>cloudy_urine</t>
+  </si>
+  <si>
+    <t>foul_smelling_urine</t>
+  </si>
+  <si>
+    <t>blood_in_urine</t>
+  </si>
+  <si>
+    <t>tired</t>
+  </si>
+  <si>
+    <t>Upper Urinary tract infection</t>
+  </si>
+  <si>
+    <t>high_temperature</t>
+  </si>
+  <si>
+    <t>pain_in_back</t>
+  </si>
+  <si>
+    <t>shivering</t>
+  </si>
+  <si>
+    <t>confusion</t>
+  </si>
+  <si>
+    <t>agitation</t>
+  </si>
+  <si>
+    <t>Psoriasis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> skin_rash</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> joint_pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> skin_peeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> silver_like_dusting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> small_dents_in_nails</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> inflammatory_nails</t>
+  </si>
+  <si>
+    <t>hepatitis A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vomiting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yellowish_skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dark_urine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nausea</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> loss_of_appetite</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abdominal_pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> diarrhoea</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mild_fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yellowing_of_eyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> muscle_pain</t>
+  </si>
+  <si>
+    <t>yellowish_skin</t>
+  </si>
+  <si>
+    <t>dark_urine</t>
+  </si>
+  <si>
+    <t>fever</t>
+  </si>
+  <si>
+    <t>Hepatitis B</t>
+  </si>
+  <si>
+    <t>upper_belly_pain</t>
+  </si>
+  <si>
+    <t>tiredness</t>
+  </si>
+  <si>
+    <t>yellowing_of_the_skin</t>
+  </si>
+  <si>
+    <t>hives</t>
+  </si>
+  <si>
+    <t>jaundice</t>
+  </si>
+  <si>
+    <t>Chronic Kidney Disease</t>
+  </si>
+  <si>
+    <t>itchy_skin</t>
+  </si>
+  <si>
+    <t>insomnia</t>
+  </si>
+  <si>
+    <t>shortness_of_breath</t>
+  </si>
+  <si>
+    <t>swollen_ankles</t>
+  </si>
+  <si>
+    <t>headaches</t>
+  </si>
+  <si>
+    <t>erectile_dysfunction</t>
+  </si>
+  <si>
+    <t>Autoimmune Diseases</t>
+  </si>
+  <si>
+    <t>stiffness</t>
+  </si>
+  <si>
+    <t>muscle_aches</t>
+  </si>
+  <si>
+    <t>skin_change</t>
   </si>
 </sst>
 </file>
@@ -544,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFD589F-1875-4119-A5A1-1BBB4D70B2D1}">
-  <dimension ref="A4:Q66"/>
+  <dimension ref="A4:Q156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2220,7 +2475,2430 @@
         <v>52</v>
       </c>
     </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" t="s">
+        <v>55</v>
+      </c>
+      <c r="H67" t="s">
+        <v>56</v>
+      </c>
+      <c r="I67" t="s">
+        <v>49</v>
+      </c>
+      <c r="J67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" t="s">
+        <v>56</v>
+      </c>
+      <c r="I68" t="s">
+        <v>49</v>
+      </c>
+      <c r="J68" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>55</v>
+      </c>
+      <c r="H69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I69" t="s">
+        <v>49</v>
+      </c>
+      <c r="J69" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" t="s">
+        <v>22</v>
+      </c>
+      <c r="F70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" t="s">
+        <v>55</v>
+      </c>
+      <c r="H70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I70" t="s">
+        <v>49</v>
+      </c>
+      <c r="J70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K70" t="s">
+        <v>48</v>
+      </c>
+      <c r="L70" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" t="s">
+        <v>22</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" t="s">
+        <v>55</v>
+      </c>
+      <c r="H71" t="s">
+        <v>56</v>
+      </c>
+      <c r="I71" t="s">
+        <v>49</v>
+      </c>
+      <c r="J71" t="s">
+        <v>17</v>
+      </c>
+      <c r="K71" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" t="s">
+        <v>22</v>
+      </c>
+      <c r="F72" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" t="s">
+        <v>55</v>
+      </c>
+      <c r="H72" t="s">
+        <v>56</v>
+      </c>
+      <c r="I72" t="s">
+        <v>49</v>
+      </c>
+      <c r="J72" t="s">
+        <v>17</v>
+      </c>
+      <c r="K72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" t="s">
+        <v>22</v>
+      </c>
+      <c r="F73" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" t="s">
+        <v>55</v>
+      </c>
+      <c r="H73" t="s">
+        <v>56</v>
+      </c>
+      <c r="I73" t="s">
+        <v>49</v>
+      </c>
+      <c r="J73" t="s">
+        <v>17</v>
+      </c>
+      <c r="K73" t="s">
+        <v>48</v>
+      </c>
+      <c r="L73" t="s">
+        <v>57</v>
+      </c>
+      <c r="M73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" t="s">
+        <v>22</v>
+      </c>
+      <c r="F74" t="s">
+        <v>18</v>
+      </c>
+      <c r="G74" t="s">
+        <v>55</v>
+      </c>
+      <c r="H74" t="s">
+        <v>56</v>
+      </c>
+      <c r="I74" t="s">
+        <v>49</v>
+      </c>
+      <c r="J74" t="s">
+        <v>17</v>
+      </c>
+      <c r="K74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" t="s">
+        <v>22</v>
+      </c>
+      <c r="F75" t="s">
+        <v>18</v>
+      </c>
+      <c r="G75" t="s">
+        <v>55</v>
+      </c>
+      <c r="H75" t="s">
+        <v>56</v>
+      </c>
+      <c r="I75" t="s">
+        <v>49</v>
+      </c>
+      <c r="J75" t="s">
+        <v>17</v>
+      </c>
+      <c r="K75" t="s">
+        <v>48</v>
+      </c>
+      <c r="L75" t="s">
+        <v>57</v>
+      </c>
+      <c r="M75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>59</v>
+      </c>
+      <c r="B76" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" t="s">
+        <v>62</v>
+      </c>
+      <c r="E76" t="s">
+        <v>63</v>
+      </c>
+      <c r="F76" t="s">
+        <v>64</v>
+      </c>
+      <c r="G76" t="s">
+        <v>65</v>
+      </c>
+      <c r="H76" t="s">
+        <v>17</v>
+      </c>
+      <c r="I76" t="s">
+        <v>66</v>
+      </c>
+      <c r="J76" t="s">
+        <v>67</v>
+      </c>
+      <c r="K76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>59</v>
+      </c>
+      <c r="B77" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" t="s">
+        <v>62</v>
+      </c>
+      <c r="E77" t="s">
+        <v>63</v>
+      </c>
+      <c r="F77" t="s">
+        <v>64</v>
+      </c>
+      <c r="G77" t="s">
+        <v>65</v>
+      </c>
+      <c r="H77" t="s">
+        <v>17</v>
+      </c>
+      <c r="I77" t="s">
+        <v>66</v>
+      </c>
+      <c r="J77" t="s">
+        <v>67</v>
+      </c>
+      <c r="K77" t="s">
+        <v>25</v>
+      </c>
+      <c r="L77" t="s">
+        <v>68</v>
+      </c>
+      <c r="M77" t="s">
+        <v>69</v>
+      </c>
+      <c r="N77" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>59</v>
+      </c>
+      <c r="B78" t="s">
+        <v>60</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E78" t="s">
+        <v>63</v>
+      </c>
+      <c r="F78" t="s">
+        <v>64</v>
+      </c>
+      <c r="G78" t="s">
+        <v>65</v>
+      </c>
+      <c r="H78" t="s">
+        <v>17</v>
+      </c>
+      <c r="I78" t="s">
+        <v>66</v>
+      </c>
+      <c r="J78" t="s">
+        <v>67</v>
+      </c>
+      <c r="K78" t="s">
+        <v>25</v>
+      </c>
+      <c r="L78" t="s">
+        <v>69</v>
+      </c>
+      <c r="M78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>59</v>
+      </c>
+      <c r="B79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C79" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" t="s">
+        <v>62</v>
+      </c>
+      <c r="E79" t="s">
+        <v>63</v>
+      </c>
+      <c r="F79" t="s">
+        <v>64</v>
+      </c>
+      <c r="G79" t="s">
+        <v>65</v>
+      </c>
+      <c r="H79" t="s">
+        <v>17</v>
+      </c>
+      <c r="I79" t="s">
+        <v>66</v>
+      </c>
+      <c r="J79" t="s">
+        <v>67</v>
+      </c>
+      <c r="K79" t="s">
+        <v>25</v>
+      </c>
+      <c r="L79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>59</v>
+      </c>
+      <c r="B80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C80" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" t="s">
+        <v>62</v>
+      </c>
+      <c r="E80" t="s">
+        <v>63</v>
+      </c>
+      <c r="F80" t="s">
+        <v>64</v>
+      </c>
+      <c r="G80" t="s">
+        <v>65</v>
+      </c>
+      <c r="H80" t="s">
+        <v>17</v>
+      </c>
+      <c r="I80" t="s">
+        <v>66</v>
+      </c>
+      <c r="J80" t="s">
+        <v>67</v>
+      </c>
+      <c r="K80" t="s">
+        <v>25</v>
+      </c>
+      <c r="L80" t="s">
+        <v>68</v>
+      </c>
+      <c r="M80" t="s">
+        <v>69</v>
+      </c>
+      <c r="N80" t="s">
+        <v>70</v>
+      </c>
+      <c r="O80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" t="s">
+        <v>60</v>
+      </c>
+      <c r="C81" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" t="s">
+        <v>62</v>
+      </c>
+      <c r="E81" t="s">
+        <v>63</v>
+      </c>
+      <c r="F81" t="s">
+        <v>64</v>
+      </c>
+      <c r="G81" t="s">
+        <v>65</v>
+      </c>
+      <c r="H81" t="s">
+        <v>17</v>
+      </c>
+      <c r="I81" t="s">
+        <v>66</v>
+      </c>
+      <c r="J81" t="s">
+        <v>67</v>
+      </c>
+      <c r="K81" t="s">
+        <v>25</v>
+      </c>
+      <c r="L81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>59</v>
+      </c>
+      <c r="B82" t="s">
+        <v>60</v>
+      </c>
+      <c r="C82" t="s">
+        <v>61</v>
+      </c>
+      <c r="D82" t="s">
+        <v>62</v>
+      </c>
+      <c r="E82" t="s">
+        <v>63</v>
+      </c>
+      <c r="F82" t="s">
+        <v>64</v>
+      </c>
+      <c r="G82" t="s">
+        <v>65</v>
+      </c>
+      <c r="H82" t="s">
+        <v>17</v>
+      </c>
+      <c r="I82" t="s">
+        <v>66</v>
+      </c>
+      <c r="J82" t="s">
+        <v>67</v>
+      </c>
+      <c r="K82" t="s">
+        <v>25</v>
+      </c>
+      <c r="L82" t="s">
+        <v>68</v>
+      </c>
+      <c r="M82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>59</v>
+      </c>
+      <c r="B83" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83" t="s">
+        <v>62</v>
+      </c>
+      <c r="E83" t="s">
+        <v>63</v>
+      </c>
+      <c r="F83" t="s">
+        <v>64</v>
+      </c>
+      <c r="G83" t="s">
+        <v>65</v>
+      </c>
+      <c r="H83" t="s">
+        <v>17</v>
+      </c>
+      <c r="I83" t="s">
+        <v>66</v>
+      </c>
+      <c r="J83" t="s">
+        <v>67</v>
+      </c>
+      <c r="K83" t="s">
+        <v>25</v>
+      </c>
+      <c r="L83" t="s">
+        <v>69</v>
+      </c>
+      <c r="M83" t="s">
+        <v>70</v>
+      </c>
+      <c r="N83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" t="s">
+        <v>74</v>
+      </c>
+      <c r="C84" t="s">
+        <v>75</v>
+      </c>
+      <c r="D84" t="s">
+        <v>76</v>
+      </c>
+      <c r="E84" t="s">
+        <v>77</v>
+      </c>
+      <c r="F84" t="s">
+        <v>78</v>
+      </c>
+      <c r="G84" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>73</v>
+      </c>
+      <c r="B85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" t="s">
+        <v>75</v>
+      </c>
+      <c r="D85" t="s">
+        <v>76</v>
+      </c>
+      <c r="E85" t="s">
+        <v>77</v>
+      </c>
+      <c r="F85" t="s">
+        <v>78</v>
+      </c>
+      <c r="G85" t="s">
+        <v>79</v>
+      </c>
+      <c r="H85" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" t="s">
+        <v>75</v>
+      </c>
+      <c r="D86" t="s">
+        <v>76</v>
+      </c>
+      <c r="E86" t="s">
+        <v>77</v>
+      </c>
+      <c r="F86" t="s">
+        <v>78</v>
+      </c>
+      <c r="G86" t="s">
+        <v>79</v>
+      </c>
+      <c r="H86" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>73</v>
+      </c>
+      <c r="B87" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" t="s">
+        <v>75</v>
+      </c>
+      <c r="D87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E87" t="s">
+        <v>77</v>
+      </c>
+      <c r="F87" t="s">
+        <v>78</v>
+      </c>
+      <c r="G87" t="s">
+        <v>79</v>
+      </c>
+      <c r="I87" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" t="s">
+        <v>75</v>
+      </c>
+      <c r="D88" t="s">
+        <v>76</v>
+      </c>
+      <c r="E88" t="s">
+        <v>77</v>
+      </c>
+      <c r="F88" t="s">
+        <v>78</v>
+      </c>
+      <c r="G88" t="s">
+        <v>79</v>
+      </c>
+      <c r="H88" t="s">
+        <v>80</v>
+      </c>
+      <c r="J88" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" t="s">
+        <v>75</v>
+      </c>
+      <c r="D89" t="s">
+        <v>76</v>
+      </c>
+      <c r="E89" t="s">
+        <v>77</v>
+      </c>
+      <c r="F89" t="s">
+        <v>78</v>
+      </c>
+      <c r="G89" t="s">
+        <v>79</v>
+      </c>
+      <c r="H89" t="s">
+        <v>80</v>
+      </c>
+      <c r="I89" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E90" t="s">
+        <v>77</v>
+      </c>
+      <c r="F90" t="s">
+        <v>78</v>
+      </c>
+      <c r="G90" t="s">
+        <v>79</v>
+      </c>
+      <c r="H90" t="s">
+        <v>81</v>
+      </c>
+      <c r="I90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>73</v>
+      </c>
+      <c r="B91" t="s">
+        <v>74</v>
+      </c>
+      <c r="C91" t="s">
+        <v>75</v>
+      </c>
+      <c r="D91" t="s">
+        <v>76</v>
+      </c>
+      <c r="E91" t="s">
+        <v>77</v>
+      </c>
+      <c r="F91" t="s">
+        <v>78</v>
+      </c>
+      <c r="G91" t="s">
+        <v>79</v>
+      </c>
+      <c r="H91" t="s">
+        <v>80</v>
+      </c>
+      <c r="I91" t="s">
+        <v>81</v>
+      </c>
+      <c r="J91" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>83</v>
+      </c>
+      <c r="B92" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" t="s">
+        <v>85</v>
+      </c>
+      <c r="D92" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92" t="s">
+        <v>87</v>
+      </c>
+      <c r="F92" t="s">
+        <v>88</v>
+      </c>
+      <c r="G92" t="s">
+        <v>89</v>
+      </c>
+      <c r="H92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>83</v>
+      </c>
+      <c r="B93" t="s">
+        <v>84</v>
+      </c>
+      <c r="C93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93" t="s">
+        <v>87</v>
+      </c>
+      <c r="F93" t="s">
+        <v>88</v>
+      </c>
+      <c r="G93" t="s">
+        <v>89</v>
+      </c>
+      <c r="H93" t="s">
+        <v>90</v>
+      </c>
+      <c r="I93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" t="s">
+        <v>87</v>
+      </c>
+      <c r="F94" t="s">
+        <v>88</v>
+      </c>
+      <c r="G94" t="s">
+        <v>89</v>
+      </c>
+      <c r="H94" t="s">
+        <v>90</v>
+      </c>
+      <c r="I94" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B95" t="s">
+        <v>84</v>
+      </c>
+      <c r="C95" t="s">
+        <v>85</v>
+      </c>
+      <c r="D95" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" t="s">
+        <v>87</v>
+      </c>
+      <c r="F95" t="s">
+        <v>88</v>
+      </c>
+      <c r="G95" t="s">
+        <v>89</v>
+      </c>
+      <c r="H95" t="s">
+        <v>90</v>
+      </c>
+      <c r="I95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>83</v>
+      </c>
+      <c r="B96" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" t="s">
+        <v>85</v>
+      </c>
+      <c r="D96" t="s">
+        <v>86</v>
+      </c>
+      <c r="E96" t="s">
+        <v>87</v>
+      </c>
+      <c r="F96" t="s">
+        <v>88</v>
+      </c>
+      <c r="G96" t="s">
+        <v>89</v>
+      </c>
+      <c r="H96" t="s">
+        <v>90</v>
+      </c>
+      <c r="I96" t="s">
+        <v>91</v>
+      </c>
+      <c r="J96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" t="s">
+        <v>84</v>
+      </c>
+      <c r="C97" t="s">
+        <v>85</v>
+      </c>
+      <c r="D97" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" t="s">
+        <v>87</v>
+      </c>
+      <c r="F97" t="s">
+        <v>88</v>
+      </c>
+      <c r="G97" t="s">
+        <v>89</v>
+      </c>
+      <c r="H97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>83</v>
+      </c>
+      <c r="B98" t="s">
+        <v>84</v>
+      </c>
+      <c r="C98" t="s">
+        <v>87</v>
+      </c>
+      <c r="D98" t="s">
+        <v>89</v>
+      </c>
+      <c r="E98" t="s">
+        <v>90</v>
+      </c>
+      <c r="F98" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99" t="s">
+        <v>84</v>
+      </c>
+      <c r="C99" t="s">
+        <v>85</v>
+      </c>
+      <c r="D99" t="s">
+        <v>86</v>
+      </c>
+      <c r="E99" t="s">
+        <v>87</v>
+      </c>
+      <c r="F99" t="s">
+        <v>88</v>
+      </c>
+      <c r="G99" t="s">
+        <v>89</v>
+      </c>
+      <c r="H99" t="s">
+        <v>90</v>
+      </c>
+      <c r="I99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>94</v>
+      </c>
+      <c r="B100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C100" t="s">
+        <v>85</v>
+      </c>
+      <c r="D100" t="s">
+        <v>86</v>
+      </c>
+      <c r="E100" t="s">
+        <v>87</v>
+      </c>
+      <c r="F100" t="s">
+        <v>88</v>
+      </c>
+      <c r="G100" t="s">
+        <v>89</v>
+      </c>
+      <c r="H100" t="s">
+        <v>90</v>
+      </c>
+      <c r="I100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>94</v>
+      </c>
+      <c r="B101" t="s">
+        <v>84</v>
+      </c>
+      <c r="C101" t="s">
+        <v>85</v>
+      </c>
+      <c r="D101" t="s">
+        <v>86</v>
+      </c>
+      <c r="E101" t="s">
+        <v>87</v>
+      </c>
+      <c r="F101" t="s">
+        <v>88</v>
+      </c>
+      <c r="G101" t="s">
+        <v>89</v>
+      </c>
+      <c r="H101" t="s">
+        <v>90</v>
+      </c>
+      <c r="I101" t="s">
+        <v>95</v>
+      </c>
+      <c r="J101" t="s">
+        <v>96</v>
+      </c>
+      <c r="K101" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" t="s">
+        <v>85</v>
+      </c>
+      <c r="D102" t="s">
+        <v>86</v>
+      </c>
+      <c r="E102" t="s">
+        <v>87</v>
+      </c>
+      <c r="F102" t="s">
+        <v>88</v>
+      </c>
+      <c r="G102" t="s">
+        <v>89</v>
+      </c>
+      <c r="H102" t="s">
+        <v>90</v>
+      </c>
+      <c r="I102" t="s">
+        <v>95</v>
+      </c>
+      <c r="J102" t="s">
+        <v>96</v>
+      </c>
+      <c r="K102" t="s">
+        <v>92</v>
+      </c>
+      <c r="L102" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103" t="s">
+        <v>85</v>
+      </c>
+      <c r="D103" t="s">
+        <v>86</v>
+      </c>
+      <c r="E103" t="s">
+        <v>87</v>
+      </c>
+      <c r="F103" t="s">
+        <v>88</v>
+      </c>
+      <c r="G103" t="s">
+        <v>89</v>
+      </c>
+      <c r="H103" t="s">
+        <v>90</v>
+      </c>
+      <c r="I103" t="s">
+        <v>95</v>
+      </c>
+      <c r="J103" t="s">
+        <v>96</v>
+      </c>
+      <c r="K103" t="s">
+        <v>92</v>
+      </c>
+      <c r="L103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>94</v>
+      </c>
+      <c r="B104" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104" t="s">
+        <v>85</v>
+      </c>
+      <c r="D104" t="s">
+        <v>86</v>
+      </c>
+      <c r="E104" t="s">
+        <v>87</v>
+      </c>
+      <c r="F104" t="s">
+        <v>88</v>
+      </c>
+      <c r="G104" t="s">
+        <v>89</v>
+      </c>
+      <c r="H104" t="s">
+        <v>90</v>
+      </c>
+      <c r="I104" t="s">
+        <v>95</v>
+      </c>
+      <c r="J104" t="s">
+        <v>96</v>
+      </c>
+      <c r="K104" t="s">
+        <v>92</v>
+      </c>
+      <c r="L104" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>94</v>
+      </c>
+      <c r="B105" t="s">
+        <v>84</v>
+      </c>
+      <c r="C105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D105" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" t="s">
+        <v>87</v>
+      </c>
+      <c r="F105" t="s">
+        <v>88</v>
+      </c>
+      <c r="G105" t="s">
+        <v>89</v>
+      </c>
+      <c r="H105" t="s">
+        <v>90</v>
+      </c>
+      <c r="I105" t="s">
+        <v>95</v>
+      </c>
+      <c r="J105" t="s">
+        <v>96</v>
+      </c>
+      <c r="K105" t="s">
+        <v>92</v>
+      </c>
+      <c r="L105" t="s">
+        <v>97</v>
+      </c>
+      <c r="M105" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>94</v>
+      </c>
+      <c r="B106" t="s">
+        <v>84</v>
+      </c>
+      <c r="C106" t="s">
+        <v>85</v>
+      </c>
+      <c r="D106" t="s">
+        <v>86</v>
+      </c>
+      <c r="E106" t="s">
+        <v>87</v>
+      </c>
+      <c r="F106" t="s">
+        <v>88</v>
+      </c>
+      <c r="G106" t="s">
+        <v>89</v>
+      </c>
+      <c r="H106" t="s">
+        <v>90</v>
+      </c>
+      <c r="I106" t="s">
+        <v>95</v>
+      </c>
+      <c r="J106" t="s">
+        <v>96</v>
+      </c>
+      <c r="K106" t="s">
+        <v>97</v>
+      </c>
+      <c r="L106" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107" t="s">
+        <v>101</v>
+      </c>
+      <c r="C107" t="s">
+        <v>102</v>
+      </c>
+      <c r="D107" t="s">
+        <v>103</v>
+      </c>
+      <c r="E107" t="s">
+        <v>104</v>
+      </c>
+      <c r="F107" t="s">
+        <v>105</v>
+      </c>
+      <c r="G107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" t="s">
+        <v>101</v>
+      </c>
+      <c r="C108" t="s">
+        <v>102</v>
+      </c>
+      <c r="D108" t="s">
+        <v>103</v>
+      </c>
+      <c r="E108" t="s">
+        <v>104</v>
+      </c>
+      <c r="F108" t="s">
+        <v>105</v>
+      </c>
+      <c r="G108" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>100</v>
+      </c>
+      <c r="B109" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" t="s">
+        <v>103</v>
+      </c>
+      <c r="D109" t="s">
+        <v>104</v>
+      </c>
+      <c r="E109" t="s">
+        <v>105</v>
+      </c>
+      <c r="F109" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>100</v>
+      </c>
+      <c r="B110" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" t="s">
+        <v>103</v>
+      </c>
+      <c r="D110" t="s">
+        <v>104</v>
+      </c>
+      <c r="E110" t="s">
+        <v>105</v>
+      </c>
+      <c r="F110" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>100</v>
+      </c>
+      <c r="B111" t="s">
+        <v>101</v>
+      </c>
+      <c r="C111" t="s">
+        <v>102</v>
+      </c>
+      <c r="D111" t="s">
+        <v>104</v>
+      </c>
+      <c r="E111" t="s">
+        <v>105</v>
+      </c>
+      <c r="F111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>100</v>
+      </c>
+      <c r="B112" t="s">
+        <v>101</v>
+      </c>
+      <c r="C112" t="s">
+        <v>102</v>
+      </c>
+      <c r="D112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E112" t="s">
+        <v>105</v>
+      </c>
+      <c r="F112" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>100</v>
+      </c>
+      <c r="B113" t="s">
+        <v>101</v>
+      </c>
+      <c r="C113" t="s">
+        <v>102</v>
+      </c>
+      <c r="D113" t="s">
+        <v>103</v>
+      </c>
+      <c r="E113" t="s">
+        <v>104</v>
+      </c>
+      <c r="F113" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>100</v>
+      </c>
+      <c r="B114" t="s">
+        <v>101</v>
+      </c>
+      <c r="C114" t="s">
+        <v>102</v>
+      </c>
+      <c r="D114" t="s">
+        <v>103</v>
+      </c>
+      <c r="E114" t="s">
+        <v>104</v>
+      </c>
+      <c r="F114" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>127</v>
+      </c>
+      <c r="B115" t="s">
+        <v>88</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E115" t="s">
+        <v>128</v>
+      </c>
+      <c r="F115" t="s">
+        <v>123</v>
+      </c>
+      <c r="G115" t="s">
+        <v>31</v>
+      </c>
+      <c r="H115" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" t="s">
+        <v>88</v>
+      </c>
+      <c r="C116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" t="s">
+        <v>92</v>
+      </c>
+      <c r="E116" t="s">
+        <v>128</v>
+      </c>
+      <c r="F116" t="s">
+        <v>123</v>
+      </c>
+      <c r="G116" t="s">
+        <v>31</v>
+      </c>
+      <c r="H116" t="s">
+        <v>129</v>
+      </c>
+      <c r="I116" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>127</v>
+      </c>
+      <c r="B117" t="s">
+        <v>88</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>92</v>
+      </c>
+      <c r="E117" t="s">
+        <v>128</v>
+      </c>
+      <c r="F117" t="s">
+        <v>123</v>
+      </c>
+      <c r="G117" t="s">
+        <v>31</v>
+      </c>
+      <c r="H117" t="s">
+        <v>129</v>
+      </c>
+      <c r="I117" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>127</v>
+      </c>
+      <c r="B118" t="s">
+        <v>88</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" t="s">
+        <v>92</v>
+      </c>
+      <c r="E118" t="s">
+        <v>128</v>
+      </c>
+      <c r="F118" t="s">
+        <v>123</v>
+      </c>
+      <c r="G118" t="s">
+        <v>31</v>
+      </c>
+      <c r="H118" t="s">
+        <v>129</v>
+      </c>
+      <c r="I118" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>127</v>
+      </c>
+      <c r="B119" t="s">
+        <v>88</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>92</v>
+      </c>
+      <c r="E119" t="s">
+        <v>128</v>
+      </c>
+      <c r="F119" t="s">
+        <v>123</v>
+      </c>
+      <c r="G119" t="s">
+        <v>31</v>
+      </c>
+      <c r="H119" t="s">
+        <v>129</v>
+      </c>
+      <c r="I119" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>127</v>
+      </c>
+      <c r="B120" t="s">
+        <v>88</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" t="s">
+        <v>92</v>
+      </c>
+      <c r="E120" t="s">
+        <v>128</v>
+      </c>
+      <c r="F120" t="s">
+        <v>123</v>
+      </c>
+      <c r="G120" t="s">
+        <v>31</v>
+      </c>
+      <c r="H120" t="s">
+        <v>129</v>
+      </c>
+      <c r="I120" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>127</v>
+      </c>
+      <c r="B121" t="s">
+        <v>88</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>92</v>
+      </c>
+      <c r="E121" t="s">
+        <v>128</v>
+      </c>
+      <c r="F121" t="s">
+        <v>123</v>
+      </c>
+      <c r="G121" t="s">
+        <v>31</v>
+      </c>
+      <c r="H121" t="s">
+        <v>129</v>
+      </c>
+      <c r="I121" t="s">
+        <v>130</v>
+      </c>
+      <c r="J121" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>127</v>
+      </c>
+      <c r="B122" t="s">
+        <v>88</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" t="s">
+        <v>92</v>
+      </c>
+      <c r="E122" t="s">
+        <v>128</v>
+      </c>
+      <c r="F122" t="s">
+        <v>123</v>
+      </c>
+      <c r="G122" t="s">
+        <v>31</v>
+      </c>
+      <c r="H122" t="s">
+        <v>129</v>
+      </c>
+      <c r="I122" t="s">
+        <v>130</v>
+      </c>
+      <c r="J122" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>127</v>
+      </c>
+      <c r="B123" t="s">
+        <v>88</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" t="s">
+        <v>92</v>
+      </c>
+      <c r="E123" t="s">
+        <v>128</v>
+      </c>
+      <c r="F123" t="s">
+        <v>123</v>
+      </c>
+      <c r="G123" t="s">
+        <v>31</v>
+      </c>
+      <c r="H123" t="s">
+        <v>129</v>
+      </c>
+      <c r="I123" t="s">
+        <v>130</v>
+      </c>
+      <c r="J123" t="s">
+        <v>132</v>
+      </c>
+      <c r="K123" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>127</v>
+      </c>
+      <c r="B124" t="s">
+        <v>88</v>
+      </c>
+      <c r="C124" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" t="s">
+        <v>92</v>
+      </c>
+      <c r="E124" t="s">
+        <v>128</v>
+      </c>
+      <c r="F124" t="s">
+        <v>123</v>
+      </c>
+      <c r="G124" t="s">
+        <v>31</v>
+      </c>
+      <c r="H124" t="s">
+        <v>129</v>
+      </c>
+      <c r="I124" t="s">
+        <v>133</v>
+      </c>
+      <c r="J124" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>88</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" t="s">
+        <v>92</v>
+      </c>
+      <c r="E125" t="s">
+        <v>128</v>
+      </c>
+      <c r="F125" t="s">
+        <v>123</v>
+      </c>
+      <c r="G125" t="s">
+        <v>31</v>
+      </c>
+      <c r="H125" t="s">
+        <v>129</v>
+      </c>
+      <c r="I125" t="s">
+        <v>130</v>
+      </c>
+      <c r="J125" t="s">
+        <v>131</v>
+      </c>
+      <c r="K125" t="s">
+        <v>132</v>
+      </c>
+      <c r="L125" t="s">
+        <v>133</v>
+      </c>
+      <c r="M125" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>127</v>
+      </c>
+      <c r="B126" t="s">
+        <v>88</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" t="s">
+        <v>92</v>
+      </c>
+      <c r="E126" t="s">
+        <v>128</v>
+      </c>
+      <c r="F126" t="s">
+        <v>123</v>
+      </c>
+      <c r="G126" t="s">
+        <v>31</v>
+      </c>
+      <c r="H126" t="s">
+        <v>129</v>
+      </c>
+      <c r="I126" t="s">
+        <v>132</v>
+      </c>
+      <c r="J126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>88</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" t="s">
+        <v>92</v>
+      </c>
+      <c r="E127" t="s">
+        <v>128</v>
+      </c>
+      <c r="F127" t="s">
+        <v>123</v>
+      </c>
+      <c r="G127" t="s">
+        <v>31</v>
+      </c>
+      <c r="H127" t="s">
+        <v>129</v>
+      </c>
+      <c r="I127" t="s">
+        <v>132</v>
+      </c>
+      <c r="J127" t="s">
+        <v>68</v>
+      </c>
+      <c r="K127" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" t="s">
+        <v>123</v>
+      </c>
+      <c r="D128" t="s">
+        <v>74</v>
+      </c>
+      <c r="E128" t="s">
+        <v>135</v>
+      </c>
+      <c r="F128" t="s">
+        <v>136</v>
+      </c>
+      <c r="G128" t="s">
+        <v>137</v>
+      </c>
+      <c r="H128" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>134</v>
+      </c>
+      <c r="B129" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" t="s">
+        <v>123</v>
+      </c>
+      <c r="D129" t="s">
+        <v>74</v>
+      </c>
+      <c r="E129" t="s">
+        <v>135</v>
+      </c>
+      <c r="F129" t="s">
+        <v>136</v>
+      </c>
+      <c r="G129" t="s">
+        <v>137</v>
+      </c>
+      <c r="H129" t="s">
+        <v>130</v>
+      </c>
+      <c r="J129" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>134</v>
+      </c>
+      <c r="B130" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130" t="s">
+        <v>123</v>
+      </c>
+      <c r="D130" t="s">
+        <v>74</v>
+      </c>
+      <c r="E130" t="s">
+        <v>135</v>
+      </c>
+      <c r="F130" t="s">
+        <v>136</v>
+      </c>
+      <c r="G130" t="s">
+        <v>137</v>
+      </c>
+      <c r="H130" t="s">
+        <v>130</v>
+      </c>
+      <c r="J130" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>134</v>
+      </c>
+      <c r="B131" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" t="s">
+        <v>123</v>
+      </c>
+      <c r="D131" t="s">
+        <v>74</v>
+      </c>
+      <c r="E131" t="s">
+        <v>135</v>
+      </c>
+      <c r="F131" t="s">
+        <v>136</v>
+      </c>
+      <c r="G131" t="s">
+        <v>137</v>
+      </c>
+      <c r="H131" t="s">
+        <v>130</v>
+      </c>
+      <c r="J131" t="s">
+        <v>120</v>
+      </c>
+      <c r="K131" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>107</v>
+      </c>
+      <c r="B145" t="s">
+        <v>102</v>
+      </c>
+      <c r="C145" t="s">
+        <v>108</v>
+      </c>
+      <c r="D145" t="s">
+        <v>109</v>
+      </c>
+      <c r="E145" t="s">
+        <v>110</v>
+      </c>
+      <c r="F145" t="s">
+        <v>111</v>
+      </c>
+      <c r="G145" t="s">
+        <v>112</v>
+      </c>
+      <c r="H145" t="s">
+        <v>113</v>
+      </c>
+      <c r="I145" t="s">
+        <v>114</v>
+      </c>
+      <c r="J145" t="s">
+        <v>115</v>
+      </c>
+      <c r="K145" t="s">
+        <v>116</v>
+      </c>
+      <c r="L145" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>107</v>
+      </c>
+      <c r="B146" t="s">
+        <v>108</v>
+      </c>
+      <c r="C146" t="s">
+        <v>109</v>
+      </c>
+      <c r="D146" t="s">
+        <v>110</v>
+      </c>
+      <c r="E146" t="s">
+        <v>111</v>
+      </c>
+      <c r="F146" t="s">
+        <v>112</v>
+      </c>
+      <c r="G146" t="s">
+        <v>113</v>
+      </c>
+      <c r="H146" t="s">
+        <v>114</v>
+      </c>
+      <c r="I146" t="s">
+        <v>120</v>
+      </c>
+      <c r="J146" t="s">
+        <v>116</v>
+      </c>
+      <c r="K146" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>107</v>
+      </c>
+      <c r="B147" t="s">
+        <v>102</v>
+      </c>
+      <c r="C147" t="s">
+        <v>109</v>
+      </c>
+      <c r="D147" t="s">
+        <v>110</v>
+      </c>
+      <c r="E147" t="s">
+        <v>111</v>
+      </c>
+      <c r="F147" t="s">
+        <v>112</v>
+      </c>
+      <c r="G147" t="s">
+        <v>113</v>
+      </c>
+      <c r="H147" t="s">
+        <v>114</v>
+      </c>
+      <c r="I147" t="s">
+        <v>120</v>
+      </c>
+      <c r="J147" t="s">
+        <v>116</v>
+      </c>
+      <c r="K147" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>107</v>
+      </c>
+      <c r="B148" t="s">
+        <v>102</v>
+      </c>
+      <c r="C148" t="s">
+        <v>108</v>
+      </c>
+      <c r="D148" t="s">
+        <v>110</v>
+      </c>
+      <c r="E148" t="s">
+        <v>111</v>
+      </c>
+      <c r="F148" t="s">
+        <v>112</v>
+      </c>
+      <c r="G148" t="s">
+        <v>113</v>
+      </c>
+      <c r="H148" t="s">
+        <v>114</v>
+      </c>
+      <c r="I148" t="s">
+        <v>120</v>
+      </c>
+      <c r="J148" t="s">
+        <v>116</v>
+      </c>
+      <c r="K148" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>107</v>
+      </c>
+      <c r="B149" t="s">
+        <v>102</v>
+      </c>
+      <c r="C149" t="s">
+        <v>108</v>
+      </c>
+      <c r="D149" t="s">
+        <v>109</v>
+      </c>
+      <c r="E149" t="s">
+        <v>111</v>
+      </c>
+      <c r="F149" t="s">
+        <v>112</v>
+      </c>
+      <c r="G149" t="s">
+        <v>113</v>
+      </c>
+      <c r="H149" t="s">
+        <v>114</v>
+      </c>
+      <c r="I149" t="s">
+        <v>120</v>
+      </c>
+      <c r="J149" t="s">
+        <v>116</v>
+      </c>
+      <c r="K149" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>107</v>
+      </c>
+      <c r="B150" t="s">
+        <v>102</v>
+      </c>
+      <c r="C150" t="s">
+        <v>108</v>
+      </c>
+      <c r="D150" t="s">
+        <v>109</v>
+      </c>
+      <c r="E150" t="s">
+        <v>110</v>
+      </c>
+      <c r="F150" t="s">
+        <v>112</v>
+      </c>
+      <c r="G150" t="s">
+        <v>113</v>
+      </c>
+      <c r="H150" t="s">
+        <v>114</v>
+      </c>
+      <c r="I150" t="s">
+        <v>120</v>
+      </c>
+      <c r="J150" t="s">
+        <v>116</v>
+      </c>
+      <c r="K150" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>107</v>
+      </c>
+      <c r="B151" t="s">
+        <v>102</v>
+      </c>
+      <c r="C151" t="s">
+        <v>108</v>
+      </c>
+      <c r="D151" t="s">
+        <v>109</v>
+      </c>
+      <c r="E151" t="s">
+        <v>110</v>
+      </c>
+      <c r="F151" t="s">
+        <v>111</v>
+      </c>
+      <c r="G151" t="s">
+        <v>113</v>
+      </c>
+      <c r="H151" t="s">
+        <v>114</v>
+      </c>
+      <c r="I151" t="s">
+        <v>120</v>
+      </c>
+      <c r="J151" t="s">
+        <v>116</v>
+      </c>
+      <c r="K151" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>121</v>
+      </c>
+      <c r="B152" t="s">
+        <v>95</v>
+      </c>
+      <c r="C152" t="s">
+        <v>122</v>
+      </c>
+      <c r="D152" t="s">
+        <v>123</v>
+      </c>
+      <c r="E152" t="s">
+        <v>118</v>
+      </c>
+      <c r="F152" t="s">
+        <v>119</v>
+      </c>
+      <c r="G152" t="s">
+        <v>124</v>
+      </c>
+      <c r="I152" t="s">
+        <v>125</v>
+      </c>
+      <c r="J152" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>121</v>
+      </c>
+      <c r="B153" t="s">
+        <v>95</v>
+      </c>
+      <c r="C153" t="s">
+        <v>122</v>
+      </c>
+      <c r="D153" t="s">
+        <v>118</v>
+      </c>
+      <c r="E153" t="s">
+        <v>119</v>
+      </c>
+      <c r="F153" t="s">
+        <v>124</v>
+      </c>
+      <c r="H153" t="s">
+        <v>125</v>
+      </c>
+      <c r="I153" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>121</v>
+      </c>
+      <c r="B154" t="s">
+        <v>95</v>
+      </c>
+      <c r="C154" t="s">
+        <v>122</v>
+      </c>
+      <c r="D154" t="s">
+        <v>118</v>
+      </c>
+      <c r="E154" t="s">
+        <v>119</v>
+      </c>
+      <c r="F154" t="s">
+        <v>124</v>
+      </c>
+      <c r="H154" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>121</v>
+      </c>
+      <c r="B155" t="s">
+        <v>95</v>
+      </c>
+      <c r="C155" t="s">
+        <v>122</v>
+      </c>
+      <c r="D155" t="s">
+        <v>118</v>
+      </c>
+      <c r="E155" t="s">
+        <v>119</v>
+      </c>
+      <c r="F155" t="s">
+        <v>124</v>
+      </c>
+      <c r="H155" t="s">
+        <v>123</v>
+      </c>
+      <c r="I155" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>121</v>
+      </c>
+      <c r="B156" t="s">
+        <v>95</v>
+      </c>
+      <c r="C156" t="s">
+        <v>122</v>
+      </c>
+      <c r="D156" t="s">
+        <v>118</v>
+      </c>
+      <c r="E156" t="s">
+        <v>119</v>
+      </c>
+      <c r="F156" t="s">
+        <v>124</v>
+      </c>
+      <c r="H156" t="s">
+        <v>125</v>
+      </c>
+      <c r="I156" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the new sentence models to the main server file
</commit_message>
<xml_diff>
--- a/Databases/Diseases.xlsx
+++ b/Databases/Diseases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIT\Level 6\FYP\FYP\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8132C9E-6FC7-4859-8D02-EF03CC4F8B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0EBBD7-6EC2-4BDB-BF0D-0A8C35C14823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBAB22AE-A4D1-47D3-AE00-9E8D5D8FBA69}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="152">
   <si>
     <t xml:space="preserve">Diabetes </t>
   </si>
@@ -357,66 +357,12 @@
     <t xml:space="preserve"> inflammatory_nails</t>
   </si>
   <si>
-    <t>hepatitis A</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vomiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> yellowish_skin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dark_urine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nausea</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> loss_of_appetite</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> abdominal_pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> diarrhoea</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mild_fever</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> yellowing_of_eyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> muscle_pain</t>
-  </si>
-  <si>
-    <t>yellowish_skin</t>
-  </si>
-  <si>
-    <t>dark_urine</t>
-  </si>
-  <si>
     <t>fever</t>
   </si>
   <si>
-    <t>Hepatitis B</t>
-  </si>
-  <si>
-    <t>upper_belly_pain</t>
-  </si>
-  <si>
     <t>tiredness</t>
   </si>
   <si>
-    <t>yellowing_of_the_skin</t>
-  </si>
-  <si>
-    <t>hives</t>
-  </si>
-  <si>
-    <t>jaundice</t>
-  </si>
-  <si>
     <t>Chronic Kidney Disease</t>
   </si>
   <si>
@@ -448,6 +394,102 @@
   </si>
   <si>
     <t>skin_change</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>vision_impairment</t>
+  </si>
+  <si>
+    <t>numbness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confusion  </t>
+  </si>
+  <si>
+    <t>trouble_walking</t>
+  </si>
+  <si>
+    <t>trouble_speaking</t>
+  </si>
+  <si>
+    <t>facial_paralysis</t>
+  </si>
+  <si>
+    <t>feeling_dizzy</t>
+  </si>
+  <si>
+    <t>falling_over</t>
+  </si>
+  <si>
+    <t>arm_paralysis</t>
+  </si>
+  <si>
+    <t>leg_paralysis</t>
+  </si>
+  <si>
+    <t>memory_loss</t>
+  </si>
+  <si>
+    <t>Coronary Artery Disease</t>
+  </si>
+  <si>
+    <t>angina</t>
+  </si>
+  <si>
+    <t>feeling_faint</t>
+  </si>
+  <si>
+    <t>pain_in_your_neck</t>
+  </si>
+  <si>
+    <t>pain_in_your_shoulders</t>
+  </si>
+  <si>
+    <t>pain_in_your_jaw</t>
+  </si>
+  <si>
+    <t>pain_in_your_arms</t>
+  </si>
+  <si>
+    <t>cold_sweat</t>
+  </si>
+  <si>
+    <t>Inflammatory Bowel Disease (IBD)</t>
+  </si>
+  <si>
+    <t>tummy_pain</t>
+  </si>
+  <si>
+    <t>diarrhea</t>
+  </si>
+  <si>
+    <t>extreme_tiredness</t>
+  </si>
+  <si>
+    <t>blood_in_stool</t>
+  </si>
+  <si>
+    <t>mucus_in_stool</t>
+  </si>
+  <si>
+    <t>skin_rash</t>
+  </si>
+  <si>
+    <t>Migraine</t>
+  </si>
+  <si>
+    <t>visual_disturbances</t>
+  </si>
+  <si>
+    <t>indigestion</t>
+  </si>
+  <si>
+    <t>changes_in_the_mood</t>
+  </si>
+  <si>
+    <t>difficulty_speaking</t>
   </si>
 </sst>
 </file>
@@ -799,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFD589F-1875-4119-A5A1-1BBB4D70B2D1}">
-  <dimension ref="A4:Q156"/>
+  <dimension ref="A4:Q176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="J184" sqref="J184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3995,7 +4037,7 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B115" t="s">
         <v>88</v>
@@ -4007,21 +4049,21 @@
         <v>92</v>
       </c>
       <c r="E115" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F115" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G115" t="s">
         <v>31</v>
       </c>
       <c r="H115" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B116" t="s">
         <v>88</v>
@@ -4033,24 +4075,24 @@
         <v>92</v>
       </c>
       <c r="E116" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F116" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G116" t="s">
         <v>31</v>
       </c>
       <c r="H116" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I116" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B117" t="s">
         <v>88</v>
@@ -4062,24 +4104,24 @@
         <v>92</v>
       </c>
       <c r="E117" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F117" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G117" t="s">
         <v>31</v>
       </c>
       <c r="H117" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I117" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B118" t="s">
         <v>88</v>
@@ -4091,24 +4133,24 @@
         <v>92</v>
       </c>
       <c r="E118" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F118" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G118" t="s">
         <v>31</v>
       </c>
       <c r="H118" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I118" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B119" t="s">
         <v>88</v>
@@ -4120,24 +4162,24 @@
         <v>92</v>
       </c>
       <c r="E119" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F119" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G119" t="s">
         <v>31</v>
       </c>
       <c r="H119" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I119" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B120" t="s">
         <v>88</v>
@@ -4149,16 +4191,16 @@
         <v>92</v>
       </c>
       <c r="E120" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F120" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G120" t="s">
         <v>31</v>
       </c>
       <c r="H120" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I120" t="s">
         <v>68</v>
@@ -4166,7 +4208,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B121" t="s">
         <v>88</v>
@@ -4178,27 +4220,27 @@
         <v>92</v>
       </c>
       <c r="E121" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F121" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G121" t="s">
         <v>31</v>
       </c>
       <c r="H121" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I121" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J121" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B122" t="s">
         <v>88</v>
@@ -4210,27 +4252,27 @@
         <v>92</v>
       </c>
       <c r="E122" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F122" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G122" t="s">
         <v>31</v>
       </c>
       <c r="H122" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I122" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J122" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B123" t="s">
         <v>88</v>
@@ -4242,22 +4284,22 @@
         <v>92</v>
       </c>
       <c r="E123" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F123" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G123" t="s">
         <v>31</v>
       </c>
       <c r="H123" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I123" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J123" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="K123" t="s">
         <v>68</v>
@@ -4265,7 +4307,7 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B124" t="s">
         <v>88</v>
@@ -4277,19 +4319,19 @@
         <v>92</v>
       </c>
       <c r="E124" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F124" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G124" t="s">
         <v>31</v>
       </c>
       <c r="H124" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I124" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="J124" t="s">
         <v>68</v>
@@ -4297,7 +4339,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B125" t="s">
         <v>88</v>
@@ -4309,28 +4351,28 @@
         <v>92</v>
       </c>
       <c r="E125" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F125" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G125" t="s">
         <v>31</v>
       </c>
       <c r="H125" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I125" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J125" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="K125" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="L125" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="M125" t="s">
         <v>68</v>
@@ -4338,7 +4380,7 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B126" t="s">
         <v>88</v>
@@ -4350,19 +4392,19 @@
         <v>92</v>
       </c>
       <c r="E126" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F126" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G126" t="s">
         <v>31</v>
       </c>
       <c r="H126" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I126" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="J126" t="s">
         <v>68</v>
@@ -4370,7 +4412,7 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B127" t="s">
         <v>88</v>
@@ -4382,106 +4424,106 @@
         <v>92</v>
       </c>
       <c r="E127" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F127" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G127" t="s">
         <v>31</v>
       </c>
       <c r="H127" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I127" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="J127" t="s">
         <v>68</v>
       </c>
       <c r="K127" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B128" t="s">
         <v>17</v>
       </c>
       <c r="C128" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D128" t="s">
         <v>74</v>
       </c>
       <c r="E128" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F128" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="G128" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="H128" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B129" t="s">
         <v>17</v>
       </c>
       <c r="C129" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D129" t="s">
         <v>74</v>
       </c>
       <c r="E129" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F129" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="G129" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="H129" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J129" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B130" t="s">
         <v>17</v>
       </c>
       <c r="C130" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D130" t="s">
         <v>74</v>
       </c>
       <c r="E130" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F130" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="G130" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="H130" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J130" t="s">
         <v>37</v>
@@ -4489,412 +4531,1228 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B131" t="s">
         <v>17</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D131" t="s">
         <v>74</v>
       </c>
       <c r="E131" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F131" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="G131" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="H131" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="J131" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="K131" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>120</v>
+      </c>
+      <c r="B132" t="s">
+        <v>121</v>
+      </c>
+      <c r="C132" t="s">
+        <v>30</v>
+      </c>
+      <c r="D132" t="s">
+        <v>122</v>
+      </c>
+      <c r="E132" t="s">
+        <v>123</v>
+      </c>
+      <c r="F132" t="s">
+        <v>124</v>
+      </c>
+      <c r="G132" t="s">
+        <v>125</v>
+      </c>
+      <c r="H132" t="s">
+        <v>126</v>
+      </c>
+      <c r="I132" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>120</v>
+      </c>
+      <c r="B133" t="s">
+        <v>121</v>
+      </c>
+      <c r="C133" t="s">
+        <v>30</v>
+      </c>
+      <c r="D133" t="s">
+        <v>122</v>
+      </c>
+      <c r="E133" t="s">
+        <v>123</v>
+      </c>
+      <c r="F133" t="s">
+        <v>124</v>
+      </c>
+      <c r="G133" t="s">
+        <v>125</v>
+      </c>
+      <c r="H133" t="s">
+        <v>126</v>
+      </c>
+      <c r="I133" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>120</v>
+      </c>
+      <c r="B134" t="s">
+        <v>121</v>
+      </c>
+      <c r="C134" t="s">
+        <v>30</v>
+      </c>
+      <c r="D134" t="s">
+        <v>122</v>
+      </c>
+      <c r="E134" t="s">
+        <v>123</v>
+      </c>
+      <c r="F134" t="s">
+        <v>124</v>
+      </c>
+      <c r="G134" t="s">
+        <v>125</v>
+      </c>
+      <c r="H134" t="s">
+        <v>129</v>
+      </c>
+      <c r="I134" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>120</v>
+      </c>
+      <c r="B135" t="s">
+        <v>121</v>
+      </c>
+      <c r="C135" t="s">
+        <v>30</v>
+      </c>
+      <c r="D135" t="s">
+        <v>122</v>
+      </c>
+      <c r="E135" t="s">
+        <v>123</v>
+      </c>
+      <c r="F135" t="s">
+        <v>124</v>
+      </c>
+      <c r="G135" t="s">
+        <v>125</v>
+      </c>
+      <c r="H135" t="s">
+        <v>129</v>
+      </c>
+      <c r="I135" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>120</v>
+      </c>
+      <c r="B136" t="s">
+        <v>121</v>
+      </c>
+      <c r="C136" t="s">
+        <v>30</v>
+      </c>
+      <c r="D136" t="s">
+        <v>122</v>
+      </c>
+      <c r="E136" t="s">
+        <v>123</v>
+      </c>
+      <c r="F136" t="s">
+        <v>124</v>
+      </c>
+      <c r="G136" t="s">
+        <v>125</v>
+      </c>
+      <c r="H136" t="s">
+        <v>130</v>
+      </c>
+      <c r="I136" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>120</v>
+      </c>
+      <c r="B137" t="s">
+        <v>121</v>
+      </c>
+      <c r="C137" t="s">
+        <v>30</v>
+      </c>
+      <c r="D137" t="s">
+        <v>122</v>
+      </c>
+      <c r="E137" t="s">
+        <v>123</v>
+      </c>
+      <c r="F137" t="s">
+        <v>124</v>
+      </c>
+      <c r="G137" t="s">
+        <v>125</v>
+      </c>
+      <c r="H137" t="s">
+        <v>130</v>
+      </c>
+      <c r="I137" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>120</v>
+      </c>
+      <c r="B138" t="s">
+        <v>121</v>
+      </c>
+      <c r="C138" t="s">
+        <v>30</v>
+      </c>
+      <c r="D138" t="s">
+        <v>122</v>
+      </c>
+      <c r="E138" t="s">
+        <v>131</v>
+      </c>
+      <c r="F138" t="s">
+        <v>124</v>
+      </c>
+      <c r="G138" t="s">
+        <v>125</v>
+      </c>
+      <c r="H138" t="s">
+        <v>126</v>
+      </c>
+      <c r="I138" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>120</v>
+      </c>
+      <c r="B139" t="s">
+        <v>121</v>
+      </c>
+      <c r="C139" t="s">
+        <v>30</v>
+      </c>
+      <c r="D139" t="s">
+        <v>122</v>
+      </c>
+      <c r="E139" t="s">
+        <v>131</v>
+      </c>
+      <c r="F139" t="s">
+        <v>124</v>
+      </c>
+      <c r="G139" t="s">
+        <v>125</v>
+      </c>
+      <c r="H139" t="s">
+        <v>126</v>
+      </c>
+      <c r="I139" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>120</v>
+      </c>
+      <c r="B140" t="s">
+        <v>121</v>
+      </c>
+      <c r="C140" t="s">
+        <v>30</v>
+      </c>
+      <c r="D140" t="s">
+        <v>122</v>
+      </c>
+      <c r="E140" t="s">
+        <v>131</v>
+      </c>
+      <c r="F140" t="s">
+        <v>124</v>
+      </c>
+      <c r="G140" t="s">
+        <v>125</v>
+      </c>
+      <c r="H140" t="s">
+        <v>129</v>
+      </c>
+      <c r="I140" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>120</v>
+      </c>
+      <c r="B141" t="s">
+        <v>121</v>
+      </c>
+      <c r="C141" t="s">
+        <v>30</v>
+      </c>
+      <c r="D141" t="s">
+        <v>122</v>
+      </c>
+      <c r="E141" t="s">
+        <v>131</v>
+      </c>
+      <c r="F141" t="s">
+        <v>124</v>
+      </c>
+      <c r="G141" t="s">
+        <v>125</v>
+      </c>
+      <c r="H141" t="s">
+        <v>129</v>
+      </c>
+      <c r="I141" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>120</v>
+      </c>
+      <c r="B142" t="s">
+        <v>121</v>
+      </c>
+      <c r="C142" t="s">
+        <v>30</v>
+      </c>
+      <c r="D142" t="s">
+        <v>122</v>
+      </c>
+      <c r="E142" t="s">
+        <v>131</v>
+      </c>
+      <c r="F142" t="s">
+        <v>124</v>
+      </c>
+      <c r="G142" t="s">
+        <v>125</v>
+      </c>
+      <c r="H142" t="s">
+        <v>130</v>
+      </c>
+      <c r="I142" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>120</v>
+      </c>
+      <c r="B143" t="s">
+        <v>121</v>
+      </c>
+      <c r="C143" t="s">
+        <v>30</v>
+      </c>
+      <c r="D143" t="s">
+        <v>122</v>
+      </c>
+      <c r="E143" t="s">
+        <v>131</v>
+      </c>
+      <c r="F143" t="s">
+        <v>124</v>
+      </c>
+      <c r="G143" t="s">
+        <v>125</v>
+      </c>
+      <c r="H143" t="s">
+        <v>130</v>
+      </c>
+      <c r="I143" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>132</v>
+      </c>
+      <c r="B144" t="s">
+        <v>133</v>
+      </c>
+      <c r="C144" t="s">
+        <v>112</v>
+      </c>
+      <c r="E144" t="s">
+        <v>134</v>
+      </c>
+      <c r="F144" t="s">
+        <v>31</v>
+      </c>
+      <c r="G144" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>132</v>
+      </c>
+      <c r="B145" t="s">
+        <v>133</v>
+      </c>
+      <c r="C145" t="s">
+        <v>112</v>
+      </c>
+      <c r="E145" t="s">
+        <v>134</v>
+      </c>
+      <c r="F145" t="s">
+        <v>31</v>
+      </c>
+      <c r="G145" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>132</v>
+      </c>
+      <c r="B146" t="s">
+        <v>133</v>
+      </c>
+      <c r="C146" t="s">
+        <v>112</v>
+      </c>
+      <c r="E146" t="s">
+        <v>134</v>
+      </c>
+      <c r="F146" t="s">
+        <v>31</v>
+      </c>
+      <c r="G146" t="s">
+        <v>135</v>
+      </c>
+      <c r="H146" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>132</v>
+      </c>
+      <c r="B147" t="s">
+        <v>133</v>
+      </c>
+      <c r="C147" t="s">
+        <v>112</v>
+      </c>
+      <c r="E147" t="s">
+        <v>134</v>
+      </c>
+      <c r="F147" t="s">
+        <v>31</v>
+      </c>
+      <c r="G147" t="s">
+        <v>136</v>
+      </c>
+      <c r="H147" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>132</v>
+      </c>
+      <c r="B148" t="s">
+        <v>133</v>
+      </c>
+      <c r="C148" t="s">
+        <v>112</v>
+      </c>
+      <c r="E148" t="s">
+        <v>134</v>
+      </c>
+      <c r="F148" t="s">
+        <v>31</v>
+      </c>
+      <c r="G148" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>132</v>
+      </c>
+      <c r="B149" t="s">
+        <v>133</v>
+      </c>
+      <c r="C149" t="s">
+        <v>112</v>
+      </c>
+      <c r="E149" t="s">
+        <v>134</v>
+      </c>
+      <c r="F149" t="s">
+        <v>31</v>
+      </c>
+      <c r="G149" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>132</v>
+      </c>
+      <c r="B150" t="s">
+        <v>133</v>
+      </c>
+      <c r="C150" t="s">
+        <v>112</v>
+      </c>
+      <c r="E150" t="s">
+        <v>134</v>
+      </c>
+      <c r="F150" t="s">
+        <v>31</v>
+      </c>
+      <c r="G150" t="s">
+        <v>135</v>
+      </c>
+      <c r="H150" t="s">
+        <v>136</v>
+      </c>
+      <c r="I150" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>132</v>
+      </c>
+      <c r="B151" t="s">
+        <v>133</v>
+      </c>
+      <c r="C151" t="s">
+        <v>112</v>
+      </c>
+      <c r="E151" t="s">
+        <v>134</v>
+      </c>
+      <c r="F151" t="s">
+        <v>31</v>
+      </c>
+      <c r="G151" t="s">
+        <v>135</v>
+      </c>
+      <c r="H151" t="s">
+        <v>136</v>
+      </c>
+      <c r="I151" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>132</v>
+      </c>
+      <c r="B152" t="s">
+        <v>133</v>
+      </c>
+      <c r="C152" t="s">
+        <v>112</v>
+      </c>
+      <c r="E152" t="s">
+        <v>134</v>
+      </c>
+      <c r="F152" t="s">
+        <v>139</v>
+      </c>
+      <c r="G152" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>132</v>
+      </c>
+      <c r="B153" t="s">
+        <v>133</v>
+      </c>
+      <c r="C153" t="s">
+        <v>112</v>
+      </c>
+      <c r="E153" t="s">
+        <v>134</v>
+      </c>
+      <c r="F153" t="s">
+        <v>139</v>
+      </c>
+      <c r="G153" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>132</v>
+      </c>
+      <c r="B154" t="s">
+        <v>133</v>
+      </c>
+      <c r="C154" t="s">
+        <v>112</v>
+      </c>
+      <c r="E154" t="s">
+        <v>134</v>
+      </c>
+      <c r="F154" t="s">
+        <v>139</v>
+      </c>
+      <c r="G154" t="s">
+        <v>135</v>
+      </c>
+      <c r="H154" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>132</v>
+      </c>
+      <c r="B155" t="s">
+        <v>133</v>
+      </c>
+      <c r="C155" t="s">
+        <v>112</v>
+      </c>
+      <c r="E155" t="s">
+        <v>134</v>
+      </c>
+      <c r="F155" t="s">
+        <v>139</v>
+      </c>
+      <c r="G155" t="s">
+        <v>136</v>
+      </c>
+      <c r="H155" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>132</v>
+      </c>
+      <c r="B156" t="s">
+        <v>133</v>
+      </c>
+      <c r="C156" t="s">
+        <v>112</v>
+      </c>
+      <c r="E156" t="s">
+        <v>134</v>
+      </c>
+      <c r="F156" t="s">
+        <v>139</v>
+      </c>
+      <c r="G156" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>132</v>
+      </c>
+      <c r="B157" t="s">
+        <v>133</v>
+      </c>
+      <c r="C157" t="s">
+        <v>112</v>
+      </c>
+      <c r="E157" t="s">
+        <v>134</v>
+      </c>
+      <c r="F157" t="s">
+        <v>139</v>
+      </c>
+      <c r="G157" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>132</v>
+      </c>
+      <c r="B158" t="s">
+        <v>133</v>
+      </c>
+      <c r="C158" t="s">
+        <v>112</v>
+      </c>
+      <c r="E158" t="s">
+        <v>134</v>
+      </c>
+      <c r="F158" t="s">
+        <v>139</v>
+      </c>
+      <c r="G158" t="s">
+        <v>135</v>
+      </c>
+      <c r="H158" t="s">
+        <v>136</v>
+      </c>
+      <c r="I158" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>132</v>
+      </c>
+      <c r="B159" t="s">
+        <v>133</v>
+      </c>
+      <c r="C159" t="s">
+        <v>112</v>
+      </c>
+      <c r="E159" t="s">
+        <v>134</v>
+      </c>
+      <c r="F159" t="s">
+        <v>139</v>
+      </c>
+      <c r="G159" t="s">
+        <v>135</v>
+      </c>
+      <c r="H159" t="s">
+        <v>136</v>
+      </c>
+      <c r="I159" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>140</v>
+      </c>
+      <c r="B160" t="s">
+        <v>141</v>
+      </c>
+      <c r="C160" t="s">
+        <v>142</v>
+      </c>
+      <c r="D160" t="s">
+        <v>37</v>
+      </c>
+      <c r="E160" t="s">
+        <v>8</v>
+      </c>
+      <c r="F160" t="s">
+        <v>143</v>
+      </c>
+      <c r="G160" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>140</v>
+      </c>
+      <c r="B161" t="s">
+        <v>141</v>
+      </c>
+      <c r="C161" t="s">
+        <v>142</v>
+      </c>
+      <c r="D161" t="s">
+        <v>37</v>
+      </c>
+      <c r="E161" t="s">
+        <v>8</v>
+      </c>
+      <c r="F161" t="s">
+        <v>143</v>
+      </c>
+      <c r="G161" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>140</v>
+      </c>
+      <c r="B162" t="s">
+        <v>141</v>
+      </c>
+      <c r="C162" t="s">
+        <v>142</v>
+      </c>
+      <c r="D162" t="s">
+        <v>37</v>
+      </c>
+      <c r="E162" t="s">
+        <v>8</v>
+      </c>
+      <c r="F162" t="s">
+        <v>143</v>
+      </c>
+      <c r="G162" t="s">
+        <v>144</v>
+      </c>
+      <c r="H162" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>140</v>
+      </c>
+      <c r="B163" t="s">
+        <v>141</v>
+      </c>
+      <c r="C163" t="s">
+        <v>142</v>
+      </c>
+      <c r="D163" t="s">
+        <v>37</v>
+      </c>
+      <c r="E163" t="s">
+        <v>8</v>
+      </c>
+      <c r="F163" t="s">
+        <v>143</v>
+      </c>
+      <c r="G163" t="s">
+        <v>145</v>
+      </c>
+      <c r="H163" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>140</v>
+      </c>
+      <c r="B164" t="s">
+        <v>141</v>
+      </c>
+      <c r="C164" t="s">
+        <v>142</v>
+      </c>
+      <c r="D164" t="s">
+        <v>37</v>
+      </c>
+      <c r="E164" t="s">
+        <v>8</v>
+      </c>
+      <c r="F164" t="s">
+        <v>143</v>
+      </c>
+      <c r="G164" t="s">
+        <v>144</v>
+      </c>
+      <c r="H164" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>140</v>
+      </c>
+      <c r="B165" t="s">
+        <v>141</v>
+      </c>
+      <c r="C165" t="s">
+        <v>142</v>
+      </c>
+      <c r="D165" t="s">
+        <v>37</v>
+      </c>
+      <c r="E165" t="s">
+        <v>8</v>
+      </c>
+      <c r="F165" t="s">
+        <v>143</v>
+      </c>
+      <c r="G165" t="s">
+        <v>145</v>
+      </c>
+      <c r="H165" t="s">
         <v>107</v>
       </c>
-      <c r="B145" t="s">
-        <v>102</v>
-      </c>
-      <c r="C145" t="s">
-        <v>108</v>
-      </c>
-      <c r="D145" t="s">
-        <v>109</v>
-      </c>
-      <c r="E145" t="s">
-        <v>110</v>
-      </c>
-      <c r="F145" t="s">
-        <v>111</v>
-      </c>
-      <c r="G145" t="s">
-        <v>112</v>
-      </c>
-      <c r="H145" t="s">
-        <v>113</v>
-      </c>
-      <c r="I145" t="s">
-        <v>114</v>
-      </c>
-      <c r="J145" t="s">
-        <v>115</v>
-      </c>
-      <c r="K145" t="s">
-        <v>116</v>
-      </c>
-      <c r="L145" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>140</v>
+      </c>
+      <c r="B166" t="s">
+        <v>141</v>
+      </c>
+      <c r="C166" t="s">
+        <v>142</v>
+      </c>
+      <c r="D166" t="s">
+        <v>37</v>
+      </c>
+      <c r="E166" t="s">
+        <v>8</v>
+      </c>
+      <c r="F166" t="s">
+        <v>143</v>
+      </c>
+      <c r="G166" t="s">
+        <v>144</v>
+      </c>
+      <c r="H166" t="s">
+        <v>74</v>
+      </c>
+      <c r="I166" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>140</v>
+      </c>
+      <c r="B167" t="s">
+        <v>141</v>
+      </c>
+      <c r="C167" t="s">
+        <v>142</v>
+      </c>
+      <c r="D167" t="s">
+        <v>37</v>
+      </c>
+      <c r="E167" t="s">
+        <v>8</v>
+      </c>
+      <c r="F167" t="s">
+        <v>143</v>
+      </c>
+      <c r="G167" t="s">
+        <v>145</v>
+      </c>
+      <c r="H167" t="s">
+        <v>146</v>
+      </c>
+      <c r="I167" t="s">
         <v>107</v>
       </c>
-      <c r="B146" t="s">
-        <v>108</v>
-      </c>
-      <c r="C146" t="s">
-        <v>109</v>
-      </c>
-      <c r="D146" t="s">
-        <v>110</v>
-      </c>
-      <c r="E146" t="s">
-        <v>111</v>
-      </c>
-      <c r="F146" t="s">
-        <v>112</v>
-      </c>
-      <c r="G146" t="s">
-        <v>113</v>
-      </c>
-      <c r="H146" t="s">
-        <v>114</v>
-      </c>
-      <c r="I146" t="s">
-        <v>120</v>
-      </c>
-      <c r="J146" t="s">
-        <v>116</v>
-      </c>
-      <c r="K146" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>140</v>
+      </c>
+      <c r="B168" t="s">
+        <v>141</v>
+      </c>
+      <c r="C168" t="s">
+        <v>142</v>
+      </c>
+      <c r="D168" t="s">
+        <v>37</v>
+      </c>
+      <c r="E168" t="s">
+        <v>8</v>
+      </c>
+      <c r="F168" t="s">
+        <v>143</v>
+      </c>
+      <c r="G168" t="s">
+        <v>144</v>
+      </c>
+      <c r="H168" t="s">
+        <v>74</v>
+      </c>
+      <c r="I168" t="s">
+        <v>50</v>
+      </c>
+      <c r="J168" t="s">
+        <v>146</v>
+      </c>
+      <c r="K168" t="s">
         <v>107</v>
       </c>
-      <c r="B147" t="s">
-        <v>102</v>
-      </c>
-      <c r="C147" t="s">
-        <v>109</v>
-      </c>
-      <c r="D147" t="s">
-        <v>110</v>
-      </c>
-      <c r="E147" t="s">
-        <v>111</v>
-      </c>
-      <c r="F147" t="s">
-        <v>112</v>
-      </c>
-      <c r="G147" t="s">
-        <v>113</v>
-      </c>
-      <c r="H147" t="s">
-        <v>114</v>
-      </c>
-      <c r="I147" t="s">
-        <v>120</v>
-      </c>
-      <c r="J147" t="s">
-        <v>116</v>
-      </c>
-      <c r="K147" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>140</v>
+      </c>
+      <c r="B169" t="s">
+        <v>141</v>
+      </c>
+      <c r="C169" t="s">
+        <v>142</v>
+      </c>
+      <c r="D169" t="s">
+        <v>37</v>
+      </c>
+      <c r="E169" t="s">
+        <v>8</v>
+      </c>
+      <c r="F169" t="s">
+        <v>143</v>
+      </c>
+      <c r="G169" t="s">
+        <v>145</v>
+      </c>
+      <c r="H169" t="s">
+        <v>74</v>
+      </c>
+      <c r="I169" t="s">
+        <v>50</v>
+      </c>
+      <c r="J169" t="s">
+        <v>146</v>
+      </c>
+      <c r="K169" t="s">
         <v>107</v>
       </c>
-      <c r="B148" t="s">
-        <v>102</v>
-      </c>
-      <c r="C148" t="s">
-        <v>108</v>
-      </c>
-      <c r="D148" t="s">
-        <v>110</v>
-      </c>
-      <c r="E148" t="s">
-        <v>111</v>
-      </c>
-      <c r="F148" t="s">
-        <v>112</v>
-      </c>
-      <c r="G148" t="s">
-        <v>113</v>
-      </c>
-      <c r="H148" t="s">
-        <v>114</v>
-      </c>
-      <c r="I148" t="s">
-        <v>120</v>
-      </c>
-      <c r="J148" t="s">
-        <v>116</v>
-      </c>
-      <c r="K148" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>107</v>
-      </c>
-      <c r="B149" t="s">
-        <v>102</v>
-      </c>
-      <c r="C149" t="s">
-        <v>108</v>
-      </c>
-      <c r="D149" t="s">
-        <v>109</v>
-      </c>
-      <c r="E149" t="s">
-        <v>111</v>
-      </c>
-      <c r="F149" t="s">
-        <v>112</v>
-      </c>
-      <c r="G149" t="s">
-        <v>113</v>
-      </c>
-      <c r="H149" t="s">
-        <v>114</v>
-      </c>
-      <c r="I149" t="s">
-        <v>120</v>
-      </c>
-      <c r="J149" t="s">
-        <v>116</v>
-      </c>
-      <c r="K149" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>107</v>
-      </c>
-      <c r="B150" t="s">
-        <v>102</v>
-      </c>
-      <c r="C150" t="s">
-        <v>108</v>
-      </c>
-      <c r="D150" t="s">
-        <v>109</v>
-      </c>
-      <c r="E150" t="s">
-        <v>110</v>
-      </c>
-      <c r="F150" t="s">
-        <v>112</v>
-      </c>
-      <c r="G150" t="s">
-        <v>113</v>
-      </c>
-      <c r="H150" t="s">
-        <v>114</v>
-      </c>
-      <c r="I150" t="s">
-        <v>120</v>
-      </c>
-      <c r="J150" t="s">
-        <v>116</v>
-      </c>
-      <c r="K150" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>107</v>
-      </c>
-      <c r="B151" t="s">
-        <v>102</v>
-      </c>
-      <c r="C151" t="s">
-        <v>108</v>
-      </c>
-      <c r="D151" t="s">
-        <v>109</v>
-      </c>
-      <c r="E151" t="s">
-        <v>110</v>
-      </c>
-      <c r="F151" t="s">
-        <v>111</v>
-      </c>
-      <c r="G151" t="s">
-        <v>113</v>
-      </c>
-      <c r="H151" t="s">
-        <v>114</v>
-      </c>
-      <c r="I151" t="s">
-        <v>120</v>
-      </c>
-      <c r="J151" t="s">
-        <v>116</v>
-      </c>
-      <c r="K151" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>121</v>
-      </c>
-      <c r="B152" t="s">
-        <v>95</v>
-      </c>
-      <c r="C152" t="s">
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>147</v>
+      </c>
+      <c r="B170" t="s">
+        <v>75</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>148</v>
+      </c>
+      <c r="E170" t="s">
+        <v>25</v>
+      </c>
+      <c r="F170" t="s">
+        <v>149</v>
+      </c>
+      <c r="G170" t="s">
+        <v>30</v>
+      </c>
+      <c r="H170" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>147</v>
+      </c>
+      <c r="B171" t="s">
+        <v>75</v>
+      </c>
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>148</v>
+      </c>
+      <c r="E171" t="s">
+        <v>25</v>
+      </c>
+      <c r="F171" t="s">
+        <v>149</v>
+      </c>
+      <c r="G171" t="s">
+        <v>30</v>
+      </c>
+      <c r="H171" t="s">
+        <v>6</v>
+      </c>
+      <c r="I171" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>147</v>
+      </c>
+      <c r="B172" t="s">
+        <v>75</v>
+      </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172" t="s">
+        <v>148</v>
+      </c>
+      <c r="E172" t="s">
+        <v>25</v>
+      </c>
+      <c r="F172" t="s">
+        <v>149</v>
+      </c>
+      <c r="G172" t="s">
+        <v>30</v>
+      </c>
+      <c r="H172" t="s">
+        <v>6</v>
+      </c>
+      <c r="I172" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>147</v>
+      </c>
+      <c r="B173" t="s">
+        <v>75</v>
+      </c>
+      <c r="C173" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>148</v>
+      </c>
+      <c r="E173" t="s">
+        <v>25</v>
+      </c>
+      <c r="F173" t="s">
+        <v>149</v>
+      </c>
+      <c r="G173" t="s">
+        <v>30</v>
+      </c>
+      <c r="H173" t="s">
+        <v>6</v>
+      </c>
+      <c r="I173" t="s">
         <v>122</v>
       </c>
-      <c r="D152" t="s">
-        <v>123</v>
-      </c>
-      <c r="E152" t="s">
-        <v>118</v>
-      </c>
-      <c r="F152" t="s">
-        <v>119</v>
-      </c>
-      <c r="G152" t="s">
-        <v>124</v>
-      </c>
-      <c r="I152" t="s">
-        <v>125</v>
-      </c>
-      <c r="J152" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>121</v>
-      </c>
-      <c r="B153" t="s">
-        <v>95</v>
-      </c>
-      <c r="C153" t="s">
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>147</v>
+      </c>
+      <c r="B174" t="s">
+        <v>75</v>
+      </c>
+      <c r="C174" t="s">
+        <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>148</v>
+      </c>
+      <c r="E174" t="s">
+        <v>25</v>
+      </c>
+      <c r="F174" t="s">
+        <v>149</v>
+      </c>
+      <c r="G174" t="s">
+        <v>30</v>
+      </c>
+      <c r="H174" t="s">
+        <v>6</v>
+      </c>
+      <c r="I174" t="s">
+        <v>150</v>
+      </c>
+      <c r="J174" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>147</v>
+      </c>
+      <c r="B175" t="s">
+        <v>75</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>148</v>
+      </c>
+      <c r="E175" t="s">
+        <v>25</v>
+      </c>
+      <c r="F175" t="s">
+        <v>149</v>
+      </c>
+      <c r="G175" t="s">
+        <v>30</v>
+      </c>
+      <c r="H175" t="s">
+        <v>6</v>
+      </c>
+      <c r="I175" t="s">
+        <v>150</v>
+      </c>
+      <c r="J175" t="s">
         <v>122</v>
       </c>
-      <c r="D153" t="s">
-        <v>118</v>
-      </c>
-      <c r="E153" t="s">
-        <v>119</v>
-      </c>
-      <c r="F153" t="s">
-        <v>124</v>
-      </c>
-      <c r="H153" t="s">
-        <v>125</v>
-      </c>
-      <c r="I153" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>121</v>
-      </c>
-      <c r="B154" t="s">
-        <v>95</v>
-      </c>
-      <c r="C154" t="s">
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>147</v>
+      </c>
+      <c r="B176" t="s">
+        <v>75</v>
+      </c>
+      <c r="C176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" t="s">
+        <v>148</v>
+      </c>
+      <c r="E176" t="s">
+        <v>25</v>
+      </c>
+      <c r="F176" t="s">
+        <v>149</v>
+      </c>
+      <c r="G176" t="s">
+        <v>30</v>
+      </c>
+      <c r="H176" t="s">
+        <v>6</v>
+      </c>
+      <c r="I176" t="s">
+        <v>150</v>
+      </c>
+      <c r="J176" t="s">
+        <v>151</v>
+      </c>
+      <c r="K176" t="s">
         <v>122</v>
-      </c>
-      <c r="D154" t="s">
-        <v>118</v>
-      </c>
-      <c r="E154" t="s">
-        <v>119</v>
-      </c>
-      <c r="F154" t="s">
-        <v>124</v>
-      </c>
-      <c r="H154" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>121</v>
-      </c>
-      <c r="B155" t="s">
-        <v>95</v>
-      </c>
-      <c r="C155" t="s">
-        <v>122</v>
-      </c>
-      <c r="D155" t="s">
-        <v>118</v>
-      </c>
-      <c r="E155" t="s">
-        <v>119</v>
-      </c>
-      <c r="F155" t="s">
-        <v>124</v>
-      </c>
-      <c r="H155" t="s">
-        <v>123</v>
-      </c>
-      <c r="I155" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>121</v>
-      </c>
-      <c r="B156" t="s">
-        <v>95</v>
-      </c>
-      <c r="C156" t="s">
-        <v>122</v>
-      </c>
-      <c r="D156" t="s">
-        <v>118</v>
-      </c>
-      <c r="E156" t="s">
-        <v>119</v>
-      </c>
-      <c r="F156" t="s">
-        <v>124</v>
-      </c>
-      <c r="H156" t="s">
-        <v>125</v>
-      </c>
-      <c r="I156" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>